<commit_message>
refactor: Bổ sung unitSalePrice vào excel
</commit_message>
<xml_diff>
--- a/assets/templates/products.xlsx
+++ b/assets/templates/products.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhnhan/Documents/Development/Projects/Flutter/sales/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58844008-7043-7641-BAAA-624375AF6C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEDBD1-0768-9140-B3EC-03473852FC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15260" yWindow="7140" windowWidth="29440" windowHeight="18880" xr2:uid="{77361D48-D46C-B140-9729-7EF8953A68D2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{77361D48-D46C-B140-9729-7EF8953A68D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="274">
   <si>
     <t>sku</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>iPhone 15</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Z Flip4 5G 128GB</t>
   </si>
   <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_10_637957658354316100_samsung-galaxy-z-flip4-tim-1.jpg", "https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_10_637957703260561099_samsung-galaxy-z-flip4-tim-3.jpg", "https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_10_637957703261029822_samsung-galaxy-z-flip4-tim-5.jpg"]</t>
@@ -744,162 +741,108 @@
     <t>Màn Hình</t>
   </si>
   <si>
-    <t>Màn hình Gaming Acer Nitro VG270 E/27 inch/FullHD (1920x1080)/IPS 100Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_1_16_638410161185929122_man-hinh-gaming-acer-nitro-vg270-e27-inch-1.jpg", "https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_1_16_638410161185772887_man-hinh-gaming-acer-nitro-vg270-e27-inch-5.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_1_16_638410161185304172_man-hinh-gaming-acer-nitro-vg270-e27-inch-3.jpg"]</t>
   </si>
   <si>
     <t>Ngồi trước không gian hiển thị của Acer Nitro VG270 E, bạn sẽ dễ dàng hòa mình vào thế giới game và phim ảnh sống động. Sản phẩm được trang bị tấm nền LCD sắc sảo rực rỡ, có độ phân giải Full HD và tần số quét 100Hz. Acer đã đưa lên chiếc màn hình gaming này rất nhiều công nghệ hỗ trợ hiển thị ưu việt.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Xiaomi G27i EU(ELA5375EU)/27 inch/FullHD (1920x1080)/FastIPS 165Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_2_19_638439406181582599_man-hinh-gaming-xiaomi-g27i-eu-ela5375eu-27-inch-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_2_19_638439406180645203_man-hinh-gaming-xiaomi-g27i-eu-ela5375eu-27-inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_2_19_638439406181894965_man-hinh-gaming-xiaomi-g27i-eu-ela5375eu-27-inch-1.jpg"]</t>
   </si>
   <si>
     <t>Ẩn trong thiết kế tối giản của màn hình Xiaomi G27i EU là hàng loạt công nghệ hiển thị ấn tượng, đáp ứng tốt nhu cầu của các game thủ. Sản phẩm được trang bị tấm nền 27 inch xịn sò với tần số quét 165Hz siêu cao, đi kèm tính năng FreeSync cao cấp, có độ sâu màu 8 bit chuyên nghiệp và tốc độ phản hồi 1ms nhanh nhạy.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Viewsonic VX2428J/23.8inch/FHD(1920x1080)/FastIPS 180Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_11_29_638368506643795061_man-hinh-gaming-viewsonic-vx2428j-23-8-inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_11_29_638368506641845244_man-hinh-gaming-viewsonic-vx2428j-23-8-inch-4.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_11_29_638368506642689395_man-hinh-gaming-viewsonic-vx2428j-23-8-inch-3.jpg"]</t>
   </si>
   <si>
     <t>Không chỉ ghi điểm bởi thiết kế công thái học ấn tượng, màn hình Viewsonic VX2428J còn đáp ứng tốt nhu cầu đặc thù của các game thủ với tần số quét 180Hz, hỗ trợ công nghệ AMD FreeSync, đạt tốc độ phản hồi 0.5ms cực ấn tượng và hỗ trợ hiển thị nội dung HDR10 trên tấm nền Fast IPS.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Acer VG240Y E/23.8inch/FullHD (1920x1080)/IPS 100Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_21_638518964146185631_nitro-vg240y-e.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_21_638518964145716888_nitro-vg240y-e-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_21_638518964146341940_nitro-vg240y-e-2.jpg"]</t>
   </si>
   <si>
     <t>Chiếc màn hình gaming 24 inch rẻ nhất thị trường hiện nay - Acer VG240Y E là lựa chọn hàng đầu cho những game thủ muốn có được trải nghiệm hình ảnh tốt với mức đầu tư hợp lý. Sản phẩm sử dụng tấm nền IPS LCD sắc nét với tần số quét 100Hz rất mượt mà, tốc độ phản hồi 1ms và độ phân giải Full HD đáp ứng tốt những nhu cầu đặc thù khi chơi game.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Samsung Odyssey G5 LS27CG552EEXXV/27 inch QHD (2560x1440)/VA 165Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_odyssey_g5_g55c_ls27cg552eexxv_5d0a72f4b6.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_odyssey_g5_g55c_ls27cg552eexxv_1_98d79db29e.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_odyssey_g5_g55c_ls27cg552eexxv_2_1aadfc88ce.png"]</t>
   </si>
   <si>
     <t>Cùng bạn hòa mình vào thế giới game theo cách đã mắt nhất, màn hình Samsung Odyssey G5 LS27CG552EEXXV không chỉ có độ phân giải QHD cực sắc nét mà còn hỗ trợ công nghệ HDR10, mang tới những khuôn hình với độ tương phản sống động. Tần số quét 165Hz và tốc độ phản hồi 1ms đáp ứng tốt những nhu cầu đặc thù mà các game thủ cần ở một chiếc màn hình chơi game.</t>
   </si>
   <si>
-    <t>Màn hình Gaming LG 24GS50F-B.ATVQ/FullHD (1920x1080)/VA 180Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/lg_24gs50f_b_atv_dc4ebebb8d.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/lg_24gs50f_b_atv_1_9acf87cad8.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/lg_24gs50f_b_atv_2_2150014ecd.png"]</t>
   </si>
   <si>
     <t>Chạm đến trải nghiệm gaming tuyệt đỉnh với màn hình LG 24GS50F-B.ATVQ. Sản phẩm không chỉ cung cấp góc nhìn sắc nét và chân thực mà còn đạt mức tần số quét lên đến 180Hz và có tốc độ phản hồi 1ms – giúp game thủ có được trải nghiệm hình ảnh mượt mà, luôn dẫn trước đối thủ ở những tình huống quyết định của game đấu.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Asus VY249HF-R/23.8 inch FullHD (1920x1080)/IPS 100hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00908831_asus_vy249hf_r_68e27750b6.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00908831_asus_vy249hf_r_1_cdabccf824.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00908831_asus_vy249hf_r_2_c1ceff5d41.png"]</t>
   </si>
   <si>
     <t>Không chỉ đáp ứng trọn vẹn nhu cầu giải trí của game thủ với loạt thông số ấn tượng như tần số quét 100Hz và tốc độ phản hồi 1ms, màn hình Asus VY249HF-R 23.8 inch còn bảo vệ mắt người dùng với công nghệ Eye Care Plus cùng bộ lọc ánh sáng xanh hiệu quả. Tấm nền IPS cung cấp góc trông ảnh rộng mở, chân thực và chi tiết.</t>
   </si>
   <si>
-    <t>Màn hình Gaming MSI G244F E2/23.8 inch (1920x1080)/IPS 180Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00907084_msi_g244f_e2_3e89b250b7.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00907084_msi_g244f_e2_1_4ed9341f5b.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/00907084_msi_g244f_e2_2_3e8218bef9.png"]</t>
   </si>
   <si>
     <t>Thổi bùng đam mê eSports của bạn với màn hình MSI G244F E2 23.8 inch cực kỳ ấn tượng. Sản phẩm có độ phân giải Full HD (1.920 x 1.080 pixels) sắc nét, đạt tần số quét lên đến 180Hz và tốc độ phản hồi 1ms nhanh nhạy. Công nghệ Adaptive-Sync sẽ đồng bộ thông số giữa màn hình và PC để game thủ luôn có được trải nghiệm trọn vẹn nhất, mượt mà nhất.</t>
   </si>
   <si>
-    <t>Màn hình Gaming MSI G244F/23.8 inch (1920x1080)/IPS 170Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_12_25_638390940306305110_man-hinh-gaming-msi-g244f-23-8-inch-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_12_25_638390940305206766_man-hinh-gaming-msi-g244f-23-8-inch-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_12_25_638390940305831695_man-hinh-gaming-msi-g244f-23-8-inch-2.jpg"]</t>
   </si>
   <si>
     <t>Với màn hình MSI G244F 23.8 inch, bạn sẽ chạm tới những trải nghiệm game ấn tượng và mãn nhãn nhất. Sản phẩm được trang bị tấm nền IPS Full HD với tần số quét lên đến 170Hz, đạt tốc độ phản hồi 1ms cực nhanh. Công nghệ AMD FreeSync sẽ tối ưu thông số để bạn có được những trải nghiệm trọn vẹn nhất.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Viewsonic VX2479-HD-Pro/24 inch/FullHD (1920x1080)/ IPS 180Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_1_638475798491807169_man-hinh-gaming-viewsonic-vx2479-hd-pro-24-inch-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_1_638475798490829994_man-hinh-gaming-viewsonic-vx2479-hd-pro-24-inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_1_638475798491099772_man-hinh-gaming-viewsonic-vx2479-hd-pro-24-inch-5.jpg"]</t>
   </si>
   <si>
     <t>Dù làm việc hay chơi game, màn hình ViewSonic VX2479-HD-Pro đều có thể đáp ứng trọn vẹn nhu cầu của bạn. Ngoài khả năng hiển thị sắc nét, sản phẩm có thể nâng cấp tần số quét lên mức 180Hz ấn tượng và đạt tốc độ phản hồi 1ms nhanh như chớp. Tấm nền SuperClear IPS cung cấp góc trông ảnh rộng mở và diễn đạt những khuôn hình rõ nét chất lượng cao.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Acer VG240Y S/23.8 inch/FHD (1920x1080)/165Hz/UM.QV0SV.S01</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2021_11_22_637731901485313843_man-hinh-acer-vg240y-s-23-8-inch-fhd-den-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2021_11_22_637731901454844816_man-hinh-acer-vg240y-s-23-8-inch-fhd-den-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2021_11_22_637731901486095126_man-hinh-acer-vg240y-s-23-8-inch-fhd-den-4.jpg"]</t>
   </si>
   <si>
     <t>Nằm trong bộ sản phẩm màn hình cao cấp của Acer, VG240Y S sở hữu tấm nền LCD với khả năng hiển thị hình ảnh sắc sảo, hỗ trợ trải nghiệm giải trí tuyệt đắc lực. Sản phẩm ghi nhận mức tần số quét thuộc hàng cao nhất trên thị trường, đồng thời hội tụ loạt công nghệ ưu việt của Acer trong lĩnh vực hiển thị hình ảnh.</t>
   </si>
   <si>
-    <t>Màn hình Gaming LG 24GQ50F-B/23.8inch/FHD (1920x1080)/165Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_7_26_637944408573196176_man-hinh-lg-27gq50f-b27-inch-5.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_7_26_637944408573352202_man-hinh-lg-27gq50f-b27-inch-4.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_7_26_637944408571789811_man-hinh-lg-27gq50f-b27-inch-3.jpg"]</t>
   </si>
   <si>
     <t>Chiếc màn hình thế hệ mới của LG – UltraGear 24GQ50F-B hội tụ những tính năng hàng đầu để đem lại trải nghiệm gaming hoàn hảo nhất cho người dùng. Không chỉ có tần số quét 165Hz siêu mượt, sản phẩm còn đem đến tốc độ phản hồi 1ms, công nghệ AMD FreeSync và thiết kế viền bao quanh siêu mỏng.</t>
   </si>
   <si>
-    <t>Màn hình Gaming Asus VG279Q3A/27 inch/FHD(1920x1080)/180Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_9_28_638315154852858789_mam-hinh-asus-vg279q3a27-inch.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_9_28_638315154855159941_mam-hinh-asus-vg279q3a27-inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2023_9_28_638315154852326157_mam-hinh-asus-vg279q3a27-inch-1.jpg"]</t>
   </si>
   <si>
     <t>Với màn hình Asus TUF VG279Q3A, bạn sẽ có được những giờ phút giải trí trọn vẹn nhất trên tấm nền 27 inch tần số quét 180Hz siêu mượt mà. Sản phẩm được trang bị những công nghệ cao cấp như AMD FreeSync và Asus Extreme Low Motion Blur Sync nhằm tối ưu hiệu suất chơi game của bạn.</t>
   </si>
   <si>
-    <t>Màn hình Đồ họa Samsung ViewFinity S7 S70D LS27D700EAEXXV/27 inch/4K(3,840 x 2,160)/IPS 60Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_viewfinity_s7_s70d_ls27d700eaexxv_972992155e.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_viewfinity_s7_s70d_ls27d700eaexxv_1_fe2493d5ad.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/samsung_viewfinity_s7_s70d_ls27d700eaexxv_2_46b6f69077.png"]</t>
   </si>
   <si>
     <t>Là phương án hỗ trợ tuyệt vời cho giới thiết kế chuyên nghiệp và các nhà sáng tạo nội dung, màn hình Samsung ViewFinity S7 S70D UHD gây ấn tượng với độ phân giải UHD sắc nét, công nghệ HDR10 giúp màu sắc được hiển thị chân thật và độ tương phản sâu. Ngoài ra, chân đế Easy Setup giúp cho quá trình lắp đặt trở nên đơn giản, nhanh chóng hơn bao giờ hết.</t>
   </si>
   <si>
-    <t>Màn hình đồ họa Asus ProArt PA248QV-P/24inch/FHD (1920x1200)/IPS 75Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_1_638501647522620037_man-hinh-do-hoa-asus-proart-pa248qv-p-24inch-5.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_1_638501647523245060_man-hinh-do-hoa-asus-proart-pa248qv-p-24inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_5_1_638501647521682560_man-hinh-do-hoa-asus-proart-pa248qv-p-24inch-3.jpg"]</t>
   </si>
   <si>
     <t>Lựa chọn màn hình tuyệt vời cho giới văn phòng và thiết kế đồ họa chuyên nghiệp, Asus ProArt PA248QV-P 24 inch gây ấn tượng với độ phân giải Full HD sắc nét, đạt 100% sRGB, có độ chính xác màu ΔE &lt; 2, tần số quét 75Hz và rất nhiều tính năng hỗ trợ chuyên dụng khác nữa.</t>
   </si>
   <si>
-    <t>Màn hình Đồ họa Asus ProArt PA278QV/27 inch/2K/75Hz/5ms</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/asus_proart_pa278qv_38f816d93e.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/asus_proart_pa278qv_1_61603435ff.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/asus_proart_pa278qv_2_4a66a18ea1.png"]</t>
   </si>
   <si>
     <t>Được xây dựng dành cho các giới thiết kế đồ họa chuyên nghiệp, màn hình Asus ProArt PA278QV đáp ứng những tiêu chuẩn khắt khe về màu sắc và có độ phân giải lên đến WQHD. Sản phẩm có khả năng kết nối linh hoạt thông qua hệ thống cổng tương tác phong phú, chân đế linh hoạt cho phép điều chỉnh độ nghiêng, xoay và chiều cao để cung cấp trải nghiệm xem thoải mái nhất.</t>
   </si>
   <si>
-    <t>Màn hình Đồ họa Dell Ultrasharp U2424H/23.8 inch/FullHD (1920x1080)/IPS 120hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/dell_ultrasharp_24_u2424h_01775635bd.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/dell_ultrasharp_24_u2424h_1_198d6fc080.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/dell_ultrasharp_24_u2424h_2_fa98972c3a.png"]</t>
   </si>
   <si>
     <t>Hãy chuyên nghiệp hóa trải nghiệm hình ảnh của bạn với Dell Ultrasharp U2424H. Độ phân giải ấn tượng và khả năng hiển thị màu sắc chính xác là những ưu điểm nổi bật nhất của sản phẩm này. Không chỉ vậy, Dell còn đem đến nhiều công nghệ bảo vệ mắt, tránh gây ảnh hưởng đến thị lực người dùng khi làm việc và giải trí nhiều giờ mỗi ngày.</t>
   </si>
   <si>
-    <t>Màn hình Đồ họa Dell UltraSharp U2422H/23.8 inch/FHD (1920 x 1080) 60Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116238685259_man-hinh-dell-ultrasharp-u2422h-trang-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116239309794_man-hinh-dell-ultrasharp-u2422h-trang-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116235872310_man-hinh-dell-ultrasharp-u2422h-trang-2.jpg"]</t>
   </si>
   <si>
@@ -909,27 +852,18 @@
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116238685259_man-hinh-dell-ultrasharp-u2422h-trang-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116239309794_man-hinh-dell-ultrasharp-u2422h-trang-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116239309794_man-hinh-dell-ultrasharp-u2422h-trang-3.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2022_8_26_637971116235872310_man-hinh-dell-ultrasharp-u2422h-trang-2.jpg"]</t>
   </si>
   <si>
-    <t>Màn hình đồ họa Samsung ViewFinity S8 LS27B800PXEXXV/27 inch 4K (3840x2160)/IPS 60Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_6_24_638548249924438254_samsung-viewfinity-s8-ls27b800pxexxv.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_6_24_638548249924282067_samsung-viewfinity-s8-ls27b800pxexxv-1.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_6_24_638548249923635690_samsung-viewfinity-s8-ls27b800pxexxv-3.jpg"]</t>
   </si>
   <si>
     <t>Với độ chuẩn màu cực cao, khả năng hiển thị sắc nét và chuyên nghiệp, màn hình Samsung ViewFinity S8 sẽ mở ra chuẩn mực trải nghiệm mới cho công việc của bạn. Sản phẩm không chỉ đáp ứng tốt các nhu cầu văn phòng thông thường mà còn hỗ trợ lý tưởng cho công việc sáng tạo, thiết kế, in ấn, thoải mái hiện thực hóa mọi ý tưởng của bạn.</t>
   </si>
   <si>
-    <t>Màn hình di động Viewsonic VA1655/15.6 inch/FullHD (1920x1080)/IPS 60Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/viewsonic_va1655_49d735cea4.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/viewsonic_va1655_1_ddde5cb38e.png","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/viewsonic_va1655_2_b0f34810ef.png"]</t>
   </si>
   <si>
     <t>Là giải pháp hiển thị cơ động và tiện lợi cho nhiều mục đích sử dụng khác nhau, màn hình ViewSonic VA1655 được thiết kế để vận hành tương thích với các dòng laptop và thiết bị di động. Sản phẩm dùng duy nhất một cáp kết nối để truyền nội dung, có thể sắp xếp với nhiều góc bố trí khác nhau. Kích cỡ nhỏ gọn và trọng lượng nhẹ đảm bảo độ linh hoạt tối ưu.</t>
   </si>
   <si>
-    <t>Màn hình Cong MSI Pro MP272C/27 inch FHD (1920x1080)/VA 75Hz</t>
-  </si>
-  <si>
     <t>["https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_26_638497524136255848_man-hinh-cong-msi-pro-mp272C-27-inch-2.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_26_638497524136255848_man-hinh-cong-msi-pro-mp272C-27-inch-5.jpg","https://cdn2.fptshop.com.vn/unsafe/750x0/filters:quality(100)/2024_4_26_638497524136255848_man-hinh-cong-msi-pro-mp272C-27-inch-3.jpg"]</t>
   </si>
   <si>
@@ -937,6 +871,75 @@
   </si>
   <si>
     <t>P00000000</t>
+  </si>
+  <si>
+    <t>unitSalePrice</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Z Flip4</t>
+  </si>
+  <si>
+    <t>Màn hình di động Viewsonic VA1655</t>
+  </si>
+  <si>
+    <t>Màn hình Cong MSI Pro MP272C</t>
+  </si>
+  <si>
+    <t>Gaming Acer Nitro VG270</t>
+  </si>
+  <si>
+    <t>Gaming Viewsonic VX2428J</t>
+  </si>
+  <si>
+    <t>Gaming Acer VG240Y E</t>
+  </si>
+  <si>
+    <t>Gaming Samsung Odyssey G5</t>
+  </si>
+  <si>
+    <t>Gaming LG 24GS50F-B.ATVQ</t>
+  </si>
+  <si>
+    <t>Gaming Asus VY249HF-R</t>
+  </si>
+  <si>
+    <t>Gaming Xiaomi G27i EU(ELA5375EU)</t>
+  </si>
+  <si>
+    <t>Gaming MSI G244F E2</t>
+  </si>
+  <si>
+    <t>Gaming MSI G244F</t>
+  </si>
+  <si>
+    <t>Gaming Viewsonic VX2479-HD-Pro</t>
+  </si>
+  <si>
+    <t>Gaming Acer VG240Y S</t>
+  </si>
+  <si>
+    <t>Gaming LG 24GQ50F-B</t>
+  </si>
+  <si>
+    <t>Gaming Asus VG279Q3A</t>
+  </si>
+  <si>
+    <t>Đồ họa Samsung ViewFinity S7 S70D</t>
+  </si>
+  <si>
+    <t>Đồ họa Asus ProArt PA248QV-P</t>
+  </si>
+  <si>
+    <t>Đồ họa Asus ProArt PA278QV</t>
+  </si>
+  <si>
+    <t>Đồ họa Dell Ultrasharp U2424H</t>
+  </si>
+  <si>
+    <t>Đồ họa Dell UltraSharp U2422H</t>
+  </si>
+  <si>
+    <t>Đồ họa Samsung ViewFinity S8</t>
   </si>
 </sst>
 </file>
@@ -1314,19 +1317,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4D8272-31BC-F547-B711-AEFCFA4EA257}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A68"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,21 +1344,24 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="372" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>49</v>
@@ -1366,1731 +1373,1999 @@
         <v>25190000</v>
       </c>
       <c r="E2" s="1">
-        <v>50</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <f>D2*1.15</f>
+        <v>28968499.999999996</v>
+      </c>
+      <c r="F2" s="1">
+        <v>50</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>11990000</v>
       </c>
       <c r="E3" s="1">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <f t="shared" ref="E3:E66" si="0">D3*1.15</f>
+        <v>13788499.999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D4" s="1">
         <v>40490000</v>
       </c>
       <c r="E4" s="1">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>46563500</v>
+      </c>
+      <c r="F4" s="1">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D5" s="1">
         <v>12990000</v>
       </c>
       <c r="E5" s="1">
-        <v>50</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>14938499.999999998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D6" s="1">
         <v>5990000</v>
       </c>
       <c r="E6" s="1">
-        <v>50</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>6888499.9999999991</v>
+      </c>
+      <c r="F6" s="1">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D7" s="1">
         <v>12490000</v>
       </c>
       <c r="E7" s="1">
-        <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>14363499.999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>9990000</v>
       </c>
       <c r="E8" s="1">
-        <v>50</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>11488500</v>
+      </c>
+      <c r="F8" s="1">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D9" s="1">
         <v>9490000</v>
       </c>
       <c r="E9" s="1">
-        <v>50</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>10913500</v>
+      </c>
+      <c r="F9" s="1">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D10" s="1">
         <v>9990000</v>
       </c>
       <c r="E10" s="1">
-        <v>50</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>11488500</v>
+      </c>
+      <c r="F10" s="1">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D11" s="1">
         <v>4390000</v>
       </c>
       <c r="E11" s="1">
-        <v>50</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>5048500</v>
+      </c>
+      <c r="F11" s="1">
+        <v>50</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I11" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="1">
         <v>7990000</v>
       </c>
       <c r="E12" s="1">
-        <v>50</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>9188500</v>
+      </c>
+      <c r="F12" s="1">
+        <v>50</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D13" s="1">
         <v>3590000</v>
       </c>
       <c r="E13" s="1">
-        <v>50</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>4128499.9999999995</v>
+      </c>
+      <c r="F13" s="1">
+        <v>50</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D14" s="1">
         <v>3090000</v>
       </c>
       <c r="E14" s="1">
-        <v>50</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>3553499.9999999995</v>
+      </c>
+      <c r="F14" s="1">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D15" s="1">
         <v>2990000</v>
       </c>
       <c r="E15" s="1">
-        <v>50</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>3438499.9999999995</v>
+      </c>
+      <c r="F15" s="1">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D16" s="1">
         <v>2790000</v>
       </c>
       <c r="E16" s="1">
-        <v>50</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>3208499.9999999995</v>
+      </c>
+      <c r="F16" s="1">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1">
         <v>990000</v>
       </c>
       <c r="E17" s="1">
-        <v>50</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>1138500</v>
+      </c>
+      <c r="F17" s="1">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D18" s="1">
         <v>650000</v>
       </c>
       <c r="E18" s="1">
-        <v>50</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>747500</v>
+      </c>
+      <c r="F18" s="1">
+        <v>50</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D19" s="1">
         <v>700000</v>
       </c>
       <c r="E19" s="1">
-        <v>50</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>804999.99999999988</v>
+      </c>
+      <c r="F19" s="1">
+        <v>50</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D20" s="1">
         <v>620000</v>
       </c>
       <c r="E20" s="1">
-        <v>50</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>713000</v>
+      </c>
+      <c r="F20" s="1">
+        <v>50</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D21" s="1">
         <v>500000</v>
       </c>
       <c r="E21" s="1">
-        <v>50</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>575000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>50</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D22" s="1">
         <v>2690000</v>
       </c>
       <c r="E22" s="1">
-        <v>50</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>3093499.9999999995</v>
+      </c>
+      <c r="F22" s="1">
+        <v>50</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D23" s="1">
         <v>5890000</v>
       </c>
       <c r="E23" s="1">
-        <v>50</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>6773499.9999999991</v>
+      </c>
+      <c r="F23" s="1">
+        <v>50</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D24" s="1">
         <v>2090000</v>
       </c>
       <c r="E24" s="1">
-        <v>50</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G24" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>2403500</v>
+      </c>
+      <c r="F24" s="1">
+        <v>50</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D25" s="1">
         <v>23890000</v>
       </c>
       <c r="E25" s="1">
-        <v>50</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>27473499.999999996</v>
+      </c>
+      <c r="F25" s="1">
+        <v>50</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" s="1">
         <v>4899000</v>
       </c>
       <c r="E26" s="1">
-        <v>50</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H26" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>5633850</v>
+      </c>
+      <c r="F26" s="1">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="D27" s="1">
         <v>5999000</v>
       </c>
       <c r="E27" s="1">
-        <v>50</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>130</v>
+        <f t="shared" si="0"/>
+        <v>6898849.9999999991</v>
+      </c>
+      <c r="F27" s="1">
+        <v>50</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D28" s="1">
         <v>24190000</v>
       </c>
       <c r="E28" s="1">
-        <v>50</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>132</v>
+        <f t="shared" si="0"/>
+        <v>27818499.999999996</v>
+      </c>
+      <c r="F28" s="1">
+        <v>50</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H28" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I28" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D29" s="1">
         <v>17990000</v>
       </c>
       <c r="E29" s="1">
-        <v>50</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>136</v>
+        <f t="shared" si="0"/>
+        <v>20688500</v>
+      </c>
+      <c r="F29" s="1">
+        <v>50</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D30" s="1">
         <v>20990000</v>
       </c>
       <c r="E30" s="1">
-        <v>50</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>139</v>
+        <f t="shared" si="0"/>
+        <v>24138499.999999996</v>
+      </c>
+      <c r="F30" s="1">
+        <v>50</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D31" s="1">
         <v>31190000</v>
       </c>
       <c r="E31" s="1">
-        <v>50</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>141</v>
+        <f t="shared" si="0"/>
+        <v>35868500</v>
+      </c>
+      <c r="F31" s="1">
+        <v>50</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D32" s="1">
         <v>33190000</v>
       </c>
       <c r="E32" s="1">
-        <v>50</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>143</v>
+        <f t="shared" si="0"/>
+        <v>38168500</v>
+      </c>
+      <c r="F32" s="1">
+        <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D33" s="1">
         <v>25990000</v>
       </c>
       <c r="E33" s="1">
-        <v>50</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>146</v>
+        <f t="shared" si="0"/>
+        <v>29888499.999999996</v>
+      </c>
+      <c r="F33" s="1">
+        <v>50</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H33" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="D34" s="1">
         <v>18490000</v>
       </c>
       <c r="E34" s="1">
-        <v>50</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>151</v>
+        <f t="shared" si="0"/>
+        <v>21263500</v>
+      </c>
+      <c r="F34" s="1">
+        <v>50</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H34" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="D35" s="1">
         <v>17990000</v>
       </c>
       <c r="E35" s="1">
-        <v>50</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>154</v>
+        <f t="shared" si="0"/>
+        <v>20688500</v>
+      </c>
+      <c r="F35" s="1">
+        <v>50</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H35" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="D36" s="1">
         <v>14990000</v>
       </c>
       <c r="E36" s="1">
-        <v>50</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>157</v>
+        <f t="shared" si="0"/>
+        <v>17238500</v>
+      </c>
+      <c r="F36" s="1">
+        <v>50</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D37" s="1">
         <v>20990000</v>
       </c>
       <c r="E37" s="1">
-        <v>50</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>139</v>
+        <f t="shared" si="0"/>
+        <v>24138499.999999996</v>
+      </c>
+      <c r="F37" s="1">
+        <v>50</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H37" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="D38" s="1">
         <v>15690000</v>
       </c>
       <c r="E38" s="1">
-        <v>50</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>160</v>
+        <f t="shared" si="0"/>
+        <v>18043500</v>
+      </c>
+      <c r="F38" s="1">
+        <v>50</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H38" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D39" s="1">
         <v>22990000</v>
       </c>
       <c r="E39" s="1">
-        <v>50</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>162</v>
+        <f t="shared" si="0"/>
+        <v>26438499.999999996</v>
+      </c>
+      <c r="F39" s="1">
+        <v>50</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H39" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="1">
         <v>10090000</v>
       </c>
       <c r="E40" s="1">
-        <v>50</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>165</v>
+        <f t="shared" si="0"/>
+        <v>11603500</v>
+      </c>
+      <c r="F40" s="1">
+        <v>50</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H40" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D41" s="1">
         <v>21990000</v>
       </c>
       <c r="E41" s="1">
-        <v>50</v>
-      </c>
-      <c r="F41" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>25288499.999999996</v>
+      </c>
+      <c r="F41" s="1">
+        <v>50</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H41" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D42" s="1">
         <v>15790000</v>
       </c>
       <c r="E42" s="1">
-        <v>50</v>
-      </c>
-      <c r="F42" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>18158500</v>
+      </c>
+      <c r="F42" s="1">
+        <v>50</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H42" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D43" s="1">
         <v>32990000</v>
       </c>
       <c r="E43" s="1">
-        <v>50</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>174</v>
+        <f t="shared" si="0"/>
+        <v>37938500</v>
+      </c>
+      <c r="F43" s="1">
+        <v>50</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H43" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="D44" s="1">
         <v>19490000</v>
       </c>
       <c r="E44" s="1">
-        <v>50</v>
-      </c>
-      <c r="F44" s="1" t="s">
+        <f t="shared" si="0"/>
+        <v>22413500</v>
+      </c>
+      <c r="F44" s="1">
+        <v>50</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H44" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="D45" s="1">
         <v>30990000</v>
       </c>
       <c r="E45" s="1">
-        <v>50</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>181</v>
+        <f t="shared" si="0"/>
+        <v>35638500</v>
+      </c>
+      <c r="F45" s="1">
+        <v>50</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H45" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D46" s="1">
         <v>23990000</v>
       </c>
       <c r="E46" s="1">
-        <v>50</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>184</v>
+        <f t="shared" si="0"/>
+        <v>27588499.999999996</v>
+      </c>
+      <c r="F46" s="1">
+        <v>50</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H46" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I46" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>208</v>
+        <v>255</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D47" s="1">
         <v>2890000</v>
       </c>
       <c r="E47" s="1">
-        <v>50</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>210</v>
+        <f t="shared" si="0"/>
+        <v>3323499.9999999995</v>
+      </c>
+      <c r="F47" s="1">
+        <v>50</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H47" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I47" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D48" s="1">
         <v>3090000</v>
       </c>
       <c r="E48" s="1">
-        <v>50</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>213</v>
+        <f t="shared" si="0"/>
+        <v>3553499.9999999995</v>
+      </c>
+      <c r="F48" s="1">
+        <v>50</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H48" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I48" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D49" s="1">
         <v>3390000</v>
       </c>
       <c r="E49" s="1">
-        <v>50</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>216</v>
+        <f t="shared" si="0"/>
+        <v>3898499.9999999995</v>
+      </c>
+      <c r="F49" s="1">
+        <v>50</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H49" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I49" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1">
         <v>2290000</v>
       </c>
       <c r="E50" s="1">
-        <v>50</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>219</v>
+        <f t="shared" si="0"/>
+        <v>2633500</v>
+      </c>
+      <c r="F50" s="1">
+        <v>50</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H50" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I50" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D51" s="1">
         <v>5290000</v>
       </c>
       <c r="E51" s="1">
-        <v>50</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>222</v>
+        <f t="shared" si="0"/>
+        <v>6083499.9999999991</v>
+      </c>
+      <c r="F51" s="1">
+        <v>50</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H51" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I51" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D52" s="1">
         <v>2890000</v>
       </c>
       <c r="E52" s="1">
-        <v>50</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>225</v>
+        <f t="shared" si="0"/>
+        <v>3323499.9999999995</v>
+      </c>
+      <c r="F52" s="1">
+        <v>50</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H52" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I52" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D53" s="1">
         <v>2090000</v>
       </c>
       <c r="E53" s="1">
-        <v>50</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>228</v>
+        <f t="shared" si="0"/>
+        <v>2403500</v>
+      </c>
+      <c r="F53" s="1">
+        <v>50</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H53" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I53" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D54" s="1">
         <v>2890000</v>
       </c>
       <c r="E54" s="1">
-        <v>50</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>231</v>
+        <f t="shared" si="0"/>
+        <v>3323499.9999999995</v>
+      </c>
+      <c r="F54" s="1">
+        <v>50</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H54" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I54" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D55" s="1">
         <v>2690000</v>
       </c>
       <c r="E55" s="1">
-        <v>50</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>234</v>
+        <f t="shared" si="0"/>
+        <v>3093499.9999999995</v>
+      </c>
+      <c r="F55" s="1">
+        <v>50</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H55" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I55" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D56" s="1">
         <v>2890000</v>
       </c>
       <c r="E56" s="1">
-        <v>50</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>237</v>
+        <f t="shared" si="0"/>
+        <v>3323499.9999999995</v>
+      </c>
+      <c r="F56" s="1">
+        <v>50</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H56" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I56" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D57" s="1">
         <v>3390000</v>
       </c>
       <c r="E57" s="1">
-        <v>50</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>240</v>
+        <f t="shared" si="0"/>
+        <v>3898499.9999999995</v>
+      </c>
+      <c r="F57" s="1">
+        <v>50</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H57" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D58" s="1">
         <v>2890000</v>
       </c>
       <c r="E58" s="1">
-        <v>50</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>243</v>
+        <f t="shared" si="0"/>
+        <v>3323499.9999999995</v>
+      </c>
+      <c r="F58" s="1">
+        <v>50</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H58" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D59" s="1">
         <v>5170000</v>
       </c>
       <c r="E59" s="1">
-        <v>50</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>246</v>
+        <f t="shared" si="0"/>
+        <v>5945500</v>
+      </c>
+      <c r="F59" s="1">
+        <v>50</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H59" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I59" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D60" s="1">
         <v>6491000</v>
       </c>
       <c r="E60" s="1">
-        <v>50</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>249</v>
+        <f t="shared" si="0"/>
+        <v>7464649.9999999991</v>
+      </c>
+      <c r="F60" s="1">
+        <v>50</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H60" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I60" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D61" s="1">
         <v>4990000</v>
       </c>
       <c r="E61" s="1">
-        <v>50</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>252</v>
+        <f t="shared" si="0"/>
+        <v>5738500</v>
+      </c>
+      <c r="F61" s="1">
+        <v>50</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H61" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I61" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="D62" s="1">
         <v>8490000</v>
       </c>
       <c r="E62" s="1">
-        <v>50</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>255</v>
+        <f t="shared" si="0"/>
+        <v>9763500</v>
+      </c>
+      <c r="F62" s="1">
+        <v>50</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H62" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I62" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="D63" s="1">
         <v>5690000</v>
       </c>
       <c r="E63" s="1">
-        <v>50</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>258</v>
+        <f t="shared" si="0"/>
+        <v>6543499.9999999991</v>
+      </c>
+      <c r="F63" s="1">
+        <v>50</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H63" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I63" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="D64" s="1">
         <v>5490000</v>
       </c>
       <c r="E64" s="1">
-        <v>50</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>261</v>
+        <f t="shared" si="0"/>
+        <v>6313499.9999999991</v>
+      </c>
+      <c r="F64" s="1">
+        <v>50</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H64" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I64" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="D65" s="1">
         <v>5490000</v>
       </c>
       <c r="E65" s="1">
-        <v>50</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>261</v>
+        <f t="shared" si="0"/>
+        <v>6313499.9999999991</v>
+      </c>
+      <c r="F65" s="1">
+        <v>50</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H65" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I65" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D66" s="1">
         <v>7090000</v>
       </c>
       <c r="E66" s="1">
-        <v>50</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>265</v>
+        <f t="shared" si="0"/>
+        <v>8153499.9999999991</v>
+      </c>
+      <c r="F66" s="1">
+        <v>50</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H66" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I66" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="D67" s="1">
         <v>3190000</v>
       </c>
       <c r="E67" s="1">
-        <v>50</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>268</v>
+        <f t="shared" ref="E67:E68" si="1">D67*1.15</f>
+        <v>3668499.9999999995</v>
+      </c>
+      <c r="F67" s="1">
+        <v>50</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H67" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I67" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D68" s="1">
         <v>2490000</v>
       </c>
       <c r="E68" s="1">
-        <v>50</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>271</v>
+        <f t="shared" si="1"/>
+        <v>2863500</v>
+      </c>
+      <c r="F68" s="1">
+        <v>50</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H68" s="1" t="b">
+        <v>249</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I68" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: Bỏ cột deleted ở excel
</commit_message>
<xml_diff>
--- a/assets/templates/products.xlsx
+++ b/assets/templates/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhnhan/Documents/Development/Projects/Flutter/sales/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEDBD1-0768-9140-B3EC-03473852FC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8202F5-E248-9546-84EB-CFD828E194C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{77361D48-D46C-B140-9729-7EF8953A68D2}"/>
   </bookViews>
@@ -35,31 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="274">
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>importPrice</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>deleted</t>
-  </si>
-  <si>
-    <t>categoryName</t>
-  </si>
-  <si>
-    <t>imageUrl</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="273">
   <si>
     <t>Điện Thoại</t>
   </si>
@@ -873,9 +849,6 @@
     <t>P00000000</t>
   </si>
   <si>
-    <t>unitSalePrice</t>
-  </si>
-  <si>
     <t>Samsung Galaxy Z Flip4</t>
   </si>
   <si>
@@ -940,6 +913,30 @@
   </si>
   <si>
     <t>Đồ họa Samsung ViewFinity S8</t>
+  </si>
+  <si>
+    <t>Mã</t>
+  </si>
+  <si>
+    <t>Tên Sản Phẩm</t>
+  </si>
+  <si>
+    <t>Hình Ảnh</t>
+  </si>
+  <si>
+    <t>Giá Nhập</t>
+  </si>
+  <si>
+    <t>Giá Bán</t>
+  </si>
+  <si>
+    <t>Số Lượng</t>
+  </si>
+  <si>
+    <t>Mô Tả</t>
+  </si>
+  <si>
+    <t>Loại Hàng</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4D8272-31BC-F547-B711-AEFCFA4EA257}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E68"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1330,44 +1327,41 @@
     <col min="7" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>268</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>270</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>271</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="372" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <v>25190000</v>
@@ -1380,24 +1374,21 @@
         <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>11990000</v>
@@ -1410,24 +1401,21 @@
         <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1">
         <v>40490000</v>
@@ -1440,24 +1428,21 @@
         <v>50</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="170" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>12990000</v>
@@ -1470,24 +1455,21 @@
         <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1">
         <v>5990000</v>
@@ -1500,24 +1482,21 @@
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1">
         <v>12490000</v>
@@ -1530,24 +1509,21 @@
         <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1">
         <v>9990000</v>
@@ -1560,24 +1536,21 @@
         <v>50</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1">
         <v>9490000</v>
@@ -1590,24 +1563,21 @@
         <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1">
         <v>9990000</v>
@@ -1620,24 +1590,21 @@
         <v>50</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1">
         <v>4390000</v>
@@ -1650,24 +1617,21 @@
         <v>50</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1">
         <v>7990000</v>
@@ -1680,24 +1644,21 @@
         <v>50</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D13" s="1">
         <v>3590000</v>
@@ -1710,24 +1671,21 @@
         <v>50</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1">
         <v>3090000</v>
@@ -1740,24 +1698,21 @@
         <v>50</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D15" s="1">
         <v>2990000</v>
@@ -1770,24 +1725,21 @@
         <v>50</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D16" s="1">
         <v>2790000</v>
@@ -1800,24 +1752,21 @@
         <v>50</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1">
         <v>990000</v>
@@ -1830,24 +1779,21 @@
         <v>50</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1">
         <v>650000</v>
@@ -1860,24 +1806,21 @@
         <v>50</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D19" s="1">
         <v>700000</v>
@@ -1890,24 +1833,21 @@
         <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1">
         <v>620000</v>
@@ -1920,24 +1860,21 @@
         <v>50</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1">
         <v>500000</v>
@@ -1950,24 +1887,21 @@
         <v>50</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1">
         <v>2690000</v>
@@ -1980,24 +1914,21 @@
         <v>50</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D23" s="1">
         <v>5890000</v>
@@ -2010,24 +1941,21 @@
         <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1">
         <v>2090000</v>
@@ -2040,24 +1968,21 @@
         <v>50</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D25" s="1">
         <v>23890000</v>
@@ -2070,24 +1995,21 @@
         <v>50</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D26" s="1">
         <v>4899000</v>
@@ -2100,24 +2022,21 @@
         <v>50</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I26" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D27" s="1">
         <v>5999000</v>
@@ -2130,24 +2049,21 @@
         <v>50</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I27" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D28" s="1">
         <v>24190000</v>
@@ -2160,24 +2076,21 @@
         <v>50</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I28" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D29" s="1">
         <v>17990000</v>
@@ -2190,24 +2103,21 @@
         <v>50</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D30" s="1">
         <v>20990000</v>
@@ -2220,24 +2130,21 @@
         <v>50</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D31" s="1">
         <v>31190000</v>
@@ -2250,24 +2157,21 @@
         <v>50</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I31" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D32" s="1">
         <v>33190000</v>
@@ -2280,24 +2184,21 @@
         <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D33" s="1">
         <v>25990000</v>
@@ -2310,24 +2211,21 @@
         <v>50</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I33" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D34" s="1">
         <v>18490000</v>
@@ -2340,24 +2238,21 @@
         <v>50</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I34" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D35" s="1">
         <v>17990000</v>
@@ -2370,24 +2265,21 @@
         <v>50</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I35" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D36" s="1">
         <v>14990000</v>
@@ -2400,24 +2292,21 @@
         <v>50</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D37" s="1">
         <v>20990000</v>
@@ -2430,24 +2319,21 @@
         <v>50</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I37" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D38" s="1">
         <v>15690000</v>
@@ -2460,24 +2346,21 @@
         <v>50</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I38" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D39" s="1">
         <v>22990000</v>
@@ -2490,24 +2373,21 @@
         <v>50</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I39" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D40" s="1">
         <v>10090000</v>
@@ -2520,24 +2400,21 @@
         <v>50</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I40" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D41" s="1">
         <v>21990000</v>
@@ -2550,24 +2427,21 @@
         <v>50</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D42" s="1">
         <v>15790000</v>
@@ -2580,24 +2454,21 @@
         <v>50</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D43" s="1">
         <v>32990000</v>
@@ -2610,24 +2481,21 @@
         <v>50</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I43" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1">
         <v>19490000</v>
@@ -2640,24 +2508,21 @@
         <v>50</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I44" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D45" s="1">
         <v>30990000</v>
@@ -2670,24 +2535,21 @@
         <v>50</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I45" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="B46" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D46" s="1">
         <v>23990000</v>
@@ -2700,24 +2562,21 @@
         <v>50</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I46" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D47" s="1">
         <v>2890000</v>
@@ -2730,24 +2589,21 @@
         <v>50</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I47" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D48" s="1">
         <v>3090000</v>
@@ -2760,24 +2616,21 @@
         <v>50</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I48" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D49" s="1">
         <v>3390000</v>
@@ -2790,24 +2643,21 @@
         <v>50</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I49" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D50" s="1">
         <v>2290000</v>
@@ -2820,24 +2670,21 @@
         <v>50</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I50" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D51" s="1">
         <v>5290000</v>
@@ -2850,24 +2697,21 @@
         <v>50</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I51" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D52" s="1">
         <v>2890000</v>
@@ -2880,24 +2724,21 @@
         <v>50</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I52" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D53" s="1">
         <v>2090000</v>
@@ -2910,24 +2751,21 @@
         <v>50</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I53" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D54" s="1">
         <v>2890000</v>
@@ -2940,24 +2778,21 @@
         <v>50</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I54" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D55" s="1">
         <v>2690000</v>
@@ -2970,24 +2805,21 @@
         <v>50</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I55" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D56" s="1">
         <v>2890000</v>
@@ -3000,24 +2832,21 @@
         <v>50</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I56" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D57" s="1">
         <v>3390000</v>
@@ -3030,24 +2859,21 @@
         <v>50</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I57" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D58" s="1">
         <v>2890000</v>
@@ -3060,24 +2886,21 @@
         <v>50</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I58" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D59" s="1">
         <v>5170000</v>
@@ -3090,24 +2913,21 @@
         <v>50</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I59" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D60" s="1">
         <v>6491000</v>
@@ -3120,24 +2940,21 @@
         <v>50</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I60" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D61" s="1">
         <v>4990000</v>
@@ -3150,24 +2967,21 @@
         <v>50</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I61" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D62" s="1">
         <v>8490000</v>
@@ -3180,24 +2994,21 @@
         <v>50</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I62" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D63" s="1">
         <v>5690000</v>
@@ -3210,24 +3021,21 @@
         <v>50</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I63" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D64" s="1">
         <v>5490000</v>
@@ -3240,24 +3048,21 @@
         <v>50</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I64" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D65" s="1">
         <v>5490000</v>
@@ -3270,24 +3075,21 @@
         <v>50</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I65" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D66" s="1">
         <v>7090000</v>
@@ -3300,24 +3102,21 @@
         <v>50</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I66" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D67" s="1">
         <v>3190000</v>
@@ -3330,24 +3129,21 @@
         <v>50</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I67" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D68" s="1">
         <v>2490000</v>
@@ -3360,13 +3156,10 @@
         <v>50</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I68" s="1" t="b">
-        <v>0</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: Cập nhật products.xlsx
</commit_message>
<xml_diff>
--- a/assets/templates/products.xlsx
+++ b/assets/templates/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhnhan/Documents/Development/Projects/Flutter/sales/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8202F5-E248-9546-84EB-CFD828E194C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548D2A3-5E8B-E743-85FD-9DA33E33DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{77361D48-D46C-B140-9729-7EF8953A68D2}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4D8272-31BC-F547-B711-AEFCFA4EA257}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="138" workbookViewId="0">
+      <selection activeCell="T66" sqref="T66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix: Cập nhật giá bán sản phẩm cho Excel
</commit_message>
<xml_diff>
--- a/assets/templates/products.xlsx
+++ b/assets/templates/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhnhan/Documents/Development/Projects/Flutter/sales/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548D2A3-5E8B-E743-85FD-9DA33E33DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CBEED9-498C-8849-AE4A-45A7739A8EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{77361D48-D46C-B140-9729-7EF8953A68D2}"/>
   </bookViews>
@@ -1316,14 +1316,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4D8272-31BC-F547-B711-AEFCFA4EA257}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="138" workbookViewId="0">
-      <selection activeCell="T66" sqref="T66"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1366,9 +1365,8 @@
       <c r="D2" s="1">
         <v>25190000</v>
       </c>
-      <c r="E2" s="1">
-        <f>D2*1.15</f>
-        <v>28968499.999999996</v>
+      <c r="E2">
+        <v>28968500</v>
       </c>
       <c r="F2" s="1">
         <v>50</v>
@@ -1393,9 +1391,8 @@
       <c r="D3" s="2">
         <v>11990000</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E66" si="0">D3*1.15</f>
-        <v>13788499.999999998</v>
+      <c r="E3">
+        <v>13788500</v>
       </c>
       <c r="F3" s="1">
         <v>50</v>
@@ -1420,8 +1417,7 @@
       <c r="D4" s="1">
         <v>40490000</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
+      <c r="E4">
         <v>46563500</v>
       </c>
       <c r="F4" s="1">
@@ -1447,9 +1443,8 @@
       <c r="D5" s="1">
         <v>12990000</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>14938499.999999998</v>
+      <c r="E5">
+        <v>14938500</v>
       </c>
       <c r="F5" s="1">
         <v>50</v>
@@ -1474,9 +1469,8 @@
       <c r="D6" s="1">
         <v>5990000</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>6888499.9999999991</v>
+      <c r="E6">
+        <v>6888500</v>
       </c>
       <c r="F6" s="1">
         <v>50</v>
@@ -1501,9 +1495,8 @@
       <c r="D7" s="1">
         <v>12490000</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>14363499.999999998</v>
+      <c r="E7">
+        <v>14363500</v>
       </c>
       <c r="F7" s="1">
         <v>50</v>
@@ -1528,8 +1521,7 @@
       <c r="D8" s="1">
         <v>9990000</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
+      <c r="E8">
         <v>11488500</v>
       </c>
       <c r="F8" s="1">
@@ -1555,8 +1547,7 @@
       <c r="D9" s="1">
         <v>9490000</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
+      <c r="E9">
         <v>10913500</v>
       </c>
       <c r="F9" s="1">
@@ -1582,8 +1573,7 @@
       <c r="D10" s="1">
         <v>9990000</v>
       </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
+      <c r="E10">
         <v>11488500</v>
       </c>
       <c r="F10" s="1">
@@ -1609,8 +1599,7 @@
       <c r="D11" s="1">
         <v>4390000</v>
       </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
+      <c r="E11">
         <v>5048500</v>
       </c>
       <c r="F11" s="1">
@@ -1636,8 +1625,7 @@
       <c r="D12" s="1">
         <v>7990000</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
+      <c r="E12">
         <v>9188500</v>
       </c>
       <c r="F12" s="1">
@@ -1663,9 +1651,8 @@
       <c r="D13" s="1">
         <v>3590000</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>4128499.9999999995</v>
+      <c r="E13">
+        <v>4128500</v>
       </c>
       <c r="F13" s="1">
         <v>50</v>
@@ -1690,9 +1677,8 @@
       <c r="D14" s="1">
         <v>3090000</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>3553499.9999999995</v>
+      <c r="E14">
+        <v>3553500</v>
       </c>
       <c r="F14" s="1">
         <v>50</v>
@@ -1717,9 +1703,8 @@
       <c r="D15" s="1">
         <v>2990000</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>3438499.9999999995</v>
+      <c r="E15">
+        <v>3438500</v>
       </c>
       <c r="F15" s="1">
         <v>50</v>
@@ -1744,9 +1729,8 @@
       <c r="D16" s="1">
         <v>2790000</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>3208499.9999999995</v>
+      <c r="E16">
+        <v>3208500</v>
       </c>
       <c r="F16" s="1">
         <v>50</v>
@@ -1771,8 +1755,7 @@
       <c r="D17" s="1">
         <v>990000</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
+      <c r="E17">
         <v>1138500</v>
       </c>
       <c r="F17" s="1">
@@ -1798,8 +1781,7 @@
       <c r="D18" s="1">
         <v>650000</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" si="0"/>
+      <c r="E18">
         <v>747500</v>
       </c>
       <c r="F18" s="1">
@@ -1825,9 +1807,8 @@
       <c r="D19" s="1">
         <v>700000</v>
       </c>
-      <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>804999.99999999988</v>
+      <c r="E19">
+        <v>805000</v>
       </c>
       <c r="F19" s="1">
         <v>50</v>
@@ -1852,8 +1833,7 @@
       <c r="D20" s="1">
         <v>620000</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="0"/>
+      <c r="E20">
         <v>713000</v>
       </c>
       <c r="F20" s="1">
@@ -1879,8 +1859,7 @@
       <c r="D21" s="1">
         <v>500000</v>
       </c>
-      <c r="E21" s="1">
-        <f t="shared" si="0"/>
+      <c r="E21">
         <v>575000</v>
       </c>
       <c r="F21" s="1">
@@ -1906,9 +1885,8 @@
       <c r="D22" s="1">
         <v>2690000</v>
       </c>
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>3093499.9999999995</v>
+      <c r="E22">
+        <v>3093500</v>
       </c>
       <c r="F22" s="1">
         <v>50</v>
@@ -1933,9 +1911,8 @@
       <c r="D23" s="1">
         <v>5890000</v>
       </c>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>6773499.9999999991</v>
+      <c r="E23">
+        <v>6773500</v>
       </c>
       <c r="F23" s="1">
         <v>50</v>
@@ -1960,8 +1937,7 @@
       <c r="D24" s="1">
         <v>2090000</v>
       </c>
-      <c r="E24" s="1">
-        <f t="shared" si="0"/>
+      <c r="E24">
         <v>2403500</v>
       </c>
       <c r="F24" s="1">
@@ -1987,9 +1963,8 @@
       <c r="D25" s="1">
         <v>23890000</v>
       </c>
-      <c r="E25" s="1">
-        <f t="shared" si="0"/>
-        <v>27473499.999999996</v>
+      <c r="E25">
+        <v>27473500</v>
       </c>
       <c r="F25" s="1">
         <v>50</v>
@@ -2014,8 +1989,7 @@
       <c r="D26" s="1">
         <v>4899000</v>
       </c>
-      <c r="E26" s="1">
-        <f t="shared" si="0"/>
+      <c r="E26">
         <v>5633850</v>
       </c>
       <c r="F26" s="1">
@@ -2041,9 +2015,8 @@
       <c r="D27" s="1">
         <v>5999000</v>
       </c>
-      <c r="E27" s="1">
-        <f t="shared" si="0"/>
-        <v>6898849.9999999991</v>
+      <c r="E27">
+        <v>6898850</v>
       </c>
       <c r="F27" s="1">
         <v>50</v>
@@ -2068,9 +2041,8 @@
       <c r="D28" s="1">
         <v>24190000</v>
       </c>
-      <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>27818499.999999996</v>
+      <c r="E28">
+        <v>27818500</v>
       </c>
       <c r="F28" s="1">
         <v>50</v>
@@ -2095,8 +2067,7 @@
       <c r="D29" s="1">
         <v>17990000</v>
       </c>
-      <c r="E29" s="1">
-        <f t="shared" si="0"/>
+      <c r="E29">
         <v>20688500</v>
       </c>
       <c r="F29" s="1">
@@ -2122,9 +2093,8 @@
       <c r="D30" s="1">
         <v>20990000</v>
       </c>
-      <c r="E30" s="1">
-        <f t="shared" si="0"/>
-        <v>24138499.999999996</v>
+      <c r="E30">
+        <v>24138500</v>
       </c>
       <c r="F30" s="1">
         <v>50</v>
@@ -2149,8 +2119,7 @@
       <c r="D31" s="1">
         <v>31190000</v>
       </c>
-      <c r="E31" s="1">
-        <f t="shared" si="0"/>
+      <c r="E31">
         <v>35868500</v>
       </c>
       <c r="F31" s="1">
@@ -2176,8 +2145,7 @@
       <c r="D32" s="1">
         <v>33190000</v>
       </c>
-      <c r="E32" s="1">
-        <f t="shared" si="0"/>
+      <c r="E32">
         <v>38168500</v>
       </c>
       <c r="F32" s="1">
@@ -2203,9 +2171,8 @@
       <c r="D33" s="1">
         <v>25990000</v>
       </c>
-      <c r="E33" s="1">
-        <f t="shared" si="0"/>
-        <v>29888499.999999996</v>
+      <c r="E33">
+        <v>29888500</v>
       </c>
       <c r="F33" s="1">
         <v>50</v>
@@ -2230,8 +2197,7 @@
       <c r="D34" s="1">
         <v>18490000</v>
       </c>
-      <c r="E34" s="1">
-        <f t="shared" si="0"/>
+      <c r="E34">
         <v>21263500</v>
       </c>
       <c r="F34" s="1">
@@ -2257,8 +2223,7 @@
       <c r="D35" s="1">
         <v>17990000</v>
       </c>
-      <c r="E35" s="1">
-        <f t="shared" si="0"/>
+      <c r="E35">
         <v>20688500</v>
       </c>
       <c r="F35" s="1">
@@ -2284,8 +2249,7 @@
       <c r="D36" s="1">
         <v>14990000</v>
       </c>
-      <c r="E36" s="1">
-        <f t="shared" si="0"/>
+      <c r="E36">
         <v>17238500</v>
       </c>
       <c r="F36" s="1">
@@ -2311,9 +2275,8 @@
       <c r="D37" s="1">
         <v>20990000</v>
       </c>
-      <c r="E37" s="1">
-        <f t="shared" si="0"/>
-        <v>24138499.999999996</v>
+      <c r="E37">
+        <v>24138500</v>
       </c>
       <c r="F37" s="1">
         <v>50</v>
@@ -2338,8 +2301,7 @@
       <c r="D38" s="1">
         <v>15690000</v>
       </c>
-      <c r="E38" s="1">
-        <f t="shared" si="0"/>
+      <c r="E38">
         <v>18043500</v>
       </c>
       <c r="F38" s="1">
@@ -2365,9 +2327,8 @@
       <c r="D39" s="1">
         <v>22990000</v>
       </c>
-      <c r="E39" s="1">
-        <f t="shared" si="0"/>
-        <v>26438499.999999996</v>
+      <c r="E39">
+        <v>26438500</v>
       </c>
       <c r="F39" s="1">
         <v>50</v>
@@ -2392,8 +2353,7 @@
       <c r="D40" s="1">
         <v>10090000</v>
       </c>
-      <c r="E40" s="1">
-        <f t="shared" si="0"/>
+      <c r="E40">
         <v>11603500</v>
       </c>
       <c r="F40" s="1">
@@ -2419,9 +2379,8 @@
       <c r="D41" s="1">
         <v>21990000</v>
       </c>
-      <c r="E41" s="1">
-        <f t="shared" si="0"/>
-        <v>25288499.999999996</v>
+      <c r="E41">
+        <v>25288500</v>
       </c>
       <c r="F41" s="1">
         <v>50</v>
@@ -2446,8 +2405,7 @@
       <c r="D42" s="1">
         <v>15790000</v>
       </c>
-      <c r="E42" s="1">
-        <f t="shared" si="0"/>
+      <c r="E42">
         <v>18158500</v>
       </c>
       <c r="F42" s="1">
@@ -2473,8 +2431,7 @@
       <c r="D43" s="1">
         <v>32990000</v>
       </c>
-      <c r="E43" s="1">
-        <f t="shared" si="0"/>
+      <c r="E43">
         <v>37938500</v>
       </c>
       <c r="F43" s="1">
@@ -2500,8 +2457,7 @@
       <c r="D44" s="1">
         <v>19490000</v>
       </c>
-      <c r="E44" s="1">
-        <f t="shared" si="0"/>
+      <c r="E44">
         <v>22413500</v>
       </c>
       <c r="F44" s="1">
@@ -2527,8 +2483,7 @@
       <c r="D45" s="1">
         <v>30990000</v>
       </c>
-      <c r="E45" s="1">
-        <f t="shared" si="0"/>
+      <c r="E45">
         <v>35638500</v>
       </c>
       <c r="F45" s="1">
@@ -2554,9 +2509,8 @@
       <c r="D46" s="1">
         <v>23990000</v>
       </c>
-      <c r="E46" s="1">
-        <f t="shared" si="0"/>
-        <v>27588499.999999996</v>
+      <c r="E46">
+        <v>27588500</v>
       </c>
       <c r="F46" s="1">
         <v>50</v>
@@ -2581,9 +2535,8 @@
       <c r="D47" s="1">
         <v>2890000</v>
       </c>
-      <c r="E47" s="1">
-        <f t="shared" si="0"/>
-        <v>3323499.9999999995</v>
+      <c r="E47">
+        <v>3323500</v>
       </c>
       <c r="F47" s="1">
         <v>50</v>
@@ -2608,9 +2561,8 @@
       <c r="D48" s="1">
         <v>3090000</v>
       </c>
-      <c r="E48" s="1">
-        <f t="shared" si="0"/>
-        <v>3553499.9999999995</v>
+      <c r="E48">
+        <v>3553500</v>
       </c>
       <c r="F48" s="1">
         <v>50</v>
@@ -2635,9 +2587,8 @@
       <c r="D49" s="1">
         <v>3390000</v>
       </c>
-      <c r="E49" s="1">
-        <f t="shared" si="0"/>
-        <v>3898499.9999999995</v>
+      <c r="E49">
+        <v>3898500</v>
       </c>
       <c r="F49" s="1">
         <v>50</v>
@@ -2662,8 +2613,7 @@
       <c r="D50" s="1">
         <v>2290000</v>
       </c>
-      <c r="E50" s="1">
-        <f t="shared" si="0"/>
+      <c r="E50">
         <v>2633500</v>
       </c>
       <c r="F50" s="1">
@@ -2689,9 +2639,8 @@
       <c r="D51" s="1">
         <v>5290000</v>
       </c>
-      <c r="E51" s="1">
-        <f t="shared" si="0"/>
-        <v>6083499.9999999991</v>
+      <c r="E51">
+        <v>6083500</v>
       </c>
       <c r="F51" s="1">
         <v>50</v>
@@ -2716,9 +2665,8 @@
       <c r="D52" s="1">
         <v>2890000</v>
       </c>
-      <c r="E52" s="1">
-        <f t="shared" si="0"/>
-        <v>3323499.9999999995</v>
+      <c r="E52">
+        <v>3323500</v>
       </c>
       <c r="F52" s="1">
         <v>50</v>
@@ -2743,8 +2691,7 @@
       <c r="D53" s="1">
         <v>2090000</v>
       </c>
-      <c r="E53" s="1">
-        <f t="shared" si="0"/>
+      <c r="E53">
         <v>2403500</v>
       </c>
       <c r="F53" s="1">
@@ -2770,9 +2717,8 @@
       <c r="D54" s="1">
         <v>2890000</v>
       </c>
-      <c r="E54" s="1">
-        <f t="shared" si="0"/>
-        <v>3323499.9999999995</v>
+      <c r="E54">
+        <v>3323500</v>
       </c>
       <c r="F54" s="1">
         <v>50</v>
@@ -2797,9 +2743,8 @@
       <c r="D55" s="1">
         <v>2690000</v>
       </c>
-      <c r="E55" s="1">
-        <f t="shared" si="0"/>
-        <v>3093499.9999999995</v>
+      <c r="E55">
+        <v>3093500</v>
       </c>
       <c r="F55" s="1">
         <v>50</v>
@@ -2824,9 +2769,8 @@
       <c r="D56" s="1">
         <v>2890000</v>
       </c>
-      <c r="E56" s="1">
-        <f t="shared" si="0"/>
-        <v>3323499.9999999995</v>
+      <c r="E56">
+        <v>3323500</v>
       </c>
       <c r="F56" s="1">
         <v>50</v>
@@ -2851,9 +2795,8 @@
       <c r="D57" s="1">
         <v>3390000</v>
       </c>
-      <c r="E57" s="1">
-        <f t="shared" si="0"/>
-        <v>3898499.9999999995</v>
+      <c r="E57">
+        <v>3898500</v>
       </c>
       <c r="F57" s="1">
         <v>50</v>
@@ -2878,9 +2821,8 @@
       <c r="D58" s="1">
         <v>2890000</v>
       </c>
-      <c r="E58" s="1">
-        <f t="shared" si="0"/>
-        <v>3323499.9999999995</v>
+      <c r="E58">
+        <v>3323500</v>
       </c>
       <c r="F58" s="1">
         <v>50</v>
@@ -2905,8 +2847,7 @@
       <c r="D59" s="1">
         <v>5170000</v>
       </c>
-      <c r="E59" s="1">
-        <f t="shared" si="0"/>
+      <c r="E59">
         <v>5945500</v>
       </c>
       <c r="F59" s="1">
@@ -2932,9 +2873,8 @@
       <c r="D60" s="1">
         <v>6491000</v>
       </c>
-      <c r="E60" s="1">
-        <f t="shared" si="0"/>
-        <v>7464649.9999999991</v>
+      <c r="E60">
+        <v>7464650</v>
       </c>
       <c r="F60" s="1">
         <v>50</v>
@@ -2959,8 +2899,7 @@
       <c r="D61" s="1">
         <v>4990000</v>
       </c>
-      <c r="E61" s="1">
-        <f t="shared" si="0"/>
+      <c r="E61">
         <v>5738500</v>
       </c>
       <c r="F61" s="1">
@@ -2986,8 +2925,7 @@
       <c r="D62" s="1">
         <v>8490000</v>
       </c>
-      <c r="E62" s="1">
-        <f t="shared" si="0"/>
+      <c r="E62">
         <v>9763500</v>
       </c>
       <c r="F62" s="1">
@@ -3013,9 +2951,8 @@
       <c r="D63" s="1">
         <v>5690000</v>
       </c>
-      <c r="E63" s="1">
-        <f t="shared" si="0"/>
-        <v>6543499.9999999991</v>
+      <c r="E63">
+        <v>6543500</v>
       </c>
       <c r="F63" s="1">
         <v>50</v>
@@ -3040,9 +2977,8 @@
       <c r="D64" s="1">
         <v>5490000</v>
       </c>
-      <c r="E64" s="1">
-        <f t="shared" si="0"/>
-        <v>6313499.9999999991</v>
+      <c r="E64">
+        <v>6313500</v>
       </c>
       <c r="F64" s="1">
         <v>50</v>
@@ -3067,9 +3003,8 @@
       <c r="D65" s="1">
         <v>5490000</v>
       </c>
-      <c r="E65" s="1">
-        <f t="shared" si="0"/>
-        <v>6313499.9999999991</v>
+      <c r="E65">
+        <v>6313500</v>
       </c>
       <c r="F65" s="1">
         <v>50</v>
@@ -3094,9 +3029,8 @@
       <c r="D66" s="1">
         <v>7090000</v>
       </c>
-      <c r="E66" s="1">
-        <f t="shared" si="0"/>
-        <v>8153499.9999999991</v>
+      <c r="E66">
+        <v>8153500</v>
       </c>
       <c r="F66" s="1">
         <v>50</v>
@@ -3121,9 +3055,8 @@
       <c r="D67" s="1">
         <v>3190000</v>
       </c>
-      <c r="E67" s="1">
-        <f t="shared" ref="E67:E68" si="1">D67*1.15</f>
-        <v>3668499.9999999995</v>
+      <c r="E67">
+        <v>3668500</v>
       </c>
       <c r="F67" s="1">
         <v>50</v>
@@ -3148,8 +3081,7 @@
       <c r="D68" s="1">
         <v>2490000</v>
       </c>
-      <c r="E68" s="1">
-        <f t="shared" si="1"/>
+      <c r="E68">
         <v>2863500</v>
       </c>
       <c r="F68" s="1">

</xml_diff>